<commit_message>
excel file didn't format properly. hopefully this fixes it
</commit_message>
<xml_diff>
--- a/run_times_book.xlsx
+++ b/run_times_book.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/2219d800601a883f/Documents/Fall 25 school/Advanced Data Structures/Project_3/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/2219d800601a883f/Documents/GitHub/ADS_Project_3/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="326" documentId="8_{49AB58A9-8AEF-447E-80E7-EF028CDA38F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{099CD8AA-08ED-4785-B1D7-CFF024845384}"/>
+  <xr:revisionPtr revIDLastSave="468" documentId="8_{49AB58A9-8AEF-447E-80E7-EF028CDA38F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{39831B53-3FA8-48C7-B119-0511874539B0}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="0" windowWidth="11712" windowHeight="13776" xr2:uid="{21D2A120-051E-4D19-BC56-DE1EFF5AFEB6}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{21D2A120-051E-4D19-BC56-DE1EFF5AFEB6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="30">
   <si>
     <t>elements to sort:</t>
   </si>
@@ -116,6 +116,15 @@
   <si>
     <t>radix</t>
   </si>
+  <si>
+    <t>MT_quick</t>
+  </si>
+  <si>
+    <t>MT_merge</t>
+  </si>
+  <si>
+    <t>MT_radix</t>
+  </si>
 </sst>
 </file>
 
@@ -130,7 +139,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -185,6 +194,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -198,7 +219,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -254,6 +275,11 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="11" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="11" fontId="0" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="11" fontId="0" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -306,7 +332,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>Runtime (ms) (log)</a:t>
+              <a:t>Runtime (ms)</a:t>
             </a:r>
             <a:r>
               <a:rPr lang="en-US" baseline="0"/>
@@ -389,38 +415,33 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$A$26:$A$35</c:f>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>Sheet1!$A$26:$A$35</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>Sheet1!$A$30:$A$35</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>5</c:v>
+                  <c:v>50000</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>50</c:v>
+                  <c:v>500000</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>500</c:v>
+                  <c:v>5000000</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>5000</c:v>
+                  <c:v>50000000</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>50000</c:v>
+                  <c:v>500000000</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>500000</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>5000000</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>50000000</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>500000000</c:v>
-                </c:pt>
-                <c:pt idx="9">
                   <c:v>5000000000</c:v>
                 </c:pt>
               </c:numCache>
@@ -428,39 +449,34 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$26:$B$35</c:f>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>Sheet1!$B$26:$B$35</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>Sheet1!$B$30:$B$35</c:f>
               <c:numCache>
                 <c:formatCode>0.00E+00</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>3.8600000000000003E-5</c:v>
+                  <c:v>86.7</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>7.7899999999999996E-4</c:v>
+                  <c:v>10000</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.38E-2</c:v>
+                  <c:v>900000</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.96</c:v>
+                  <c:v>900000</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>86.7</c:v>
+                  <c:v>900000</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>10000</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>90000</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>90000</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>90000</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>90000</c:v>
+                  <c:v>900000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -500,38 +516,33 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$A$26:$A$35</c:f>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>Sheet1!$A$26:$A$35</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>Sheet1!$A$30:$A$35</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>5</c:v>
+                  <c:v>50000</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>50</c:v>
+                  <c:v>500000</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>500</c:v>
+                  <c:v>5000000</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>5000</c:v>
+                  <c:v>50000000</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>50000</c:v>
+                  <c:v>500000000</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>500000</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>5000000</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>50000000</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>500000000</c:v>
-                </c:pt>
-                <c:pt idx="9">
                   <c:v>5000000000</c:v>
                 </c:pt>
               </c:numCache>
@@ -539,39 +550,34 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$C$26:$C$35</c:f>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>Sheet1!$C$26:$C$35</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>Sheet1!$C$30:$C$35</c:f>
               <c:numCache>
                 <c:formatCode>0.00E+00</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>4.4400000000000002E-5</c:v>
+                  <c:v>264</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>6.3000000000000003E-4</c:v>
+                  <c:v>25400</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4.0800000000000003E-2</c:v>
+                  <c:v>900000</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2.76</c:v>
+                  <c:v>900000</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>264</c:v>
+                  <c:v>900000</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>25400</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>90000</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>90000</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>90000</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>90000</c:v>
+                  <c:v>900000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -613,38 +619,33 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$A$26:$A$35</c:f>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>Sheet1!$A$26:$A$35</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>Sheet1!$A$30:$A$35</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>5</c:v>
+                  <c:v>50000</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>50</c:v>
+                  <c:v>500000</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>500</c:v>
+                  <c:v>5000000</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>5000</c:v>
+                  <c:v>50000000</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>50000</c:v>
+                  <c:v>500000000</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>500000</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>5000000</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>50000000</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>500000000</c:v>
-                </c:pt>
-                <c:pt idx="9">
                   <c:v>5000000000</c:v>
                 </c:pt>
               </c:numCache>
@@ -652,39 +653,34 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$D$26:$D$35</c:f>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>Sheet1!$D$26:$D$35</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>Sheet1!$D$30:$D$35</c:f>
               <c:numCache>
                 <c:formatCode>0.00E+00</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>4.4100000000000001E-5</c:v>
+                  <c:v>3.7</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4.3399999999999998E-4</c:v>
+                  <c:v>49.3</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>6.9800000000000001E-3</c:v>
+                  <c:v>626</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.25600000000000001</c:v>
+                  <c:v>82800</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3.7</c:v>
+                  <c:v>900000</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>49.3</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>626</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>82800</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>90000</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>90000</c:v>
+                  <c:v>900000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -726,38 +722,33 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$A$26:$A$35</c:f>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>Sheet1!$A$26:$A$35</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>Sheet1!$A$30:$A$35</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>5</c:v>
+                  <c:v>50000</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>50</c:v>
+                  <c:v>500000</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>500</c:v>
+                  <c:v>5000000</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>5000</c:v>
+                  <c:v>50000000</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>50000</c:v>
+                  <c:v>500000000</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>500000</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>5000000</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>50000000</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>500000000</c:v>
-                </c:pt>
-                <c:pt idx="9">
                   <c:v>5000000000</c:v>
                 </c:pt>
               </c:numCache>
@@ -765,39 +756,34 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$E$26:$E$35</c:f>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>Sheet1!$E$26:$E$35</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>Sheet1!$E$30:$E$35</c:f>
               <c:numCache>
                 <c:formatCode>0.00E+00</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>3.0599999999999998E-5</c:v>
+                  <c:v>1.83</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4.4099999999999999E-4</c:v>
+                  <c:v>9.84</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>5.3E-3</c:v>
+                  <c:v>604</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.121</c:v>
+                  <c:v>30800</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.83</c:v>
+                  <c:v>900000</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>9.84</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>604</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>30800</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>90000</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>90000</c:v>
+                  <c:v>900000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -839,38 +825,33 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$A$26:$A$35</c:f>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>Sheet1!$A$26:$A$35</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>Sheet1!$A$30:$A$35</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>5</c:v>
+                  <c:v>50000</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>50</c:v>
+                  <c:v>500000</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>500</c:v>
+                  <c:v>5000000</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>5000</c:v>
+                  <c:v>50000000</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>50000</c:v>
+                  <c:v>500000000</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>500000</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>5000000</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>50000000</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>500000000</c:v>
-                </c:pt>
-                <c:pt idx="9">
                   <c:v>5000000000</c:v>
                 </c:pt>
               </c:numCache>
@@ -878,39 +859,34 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$F$26:$F$35</c:f>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>Sheet1!$F$26:$F$35</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>Sheet1!$F$30:$F$35</c:f>
               <c:numCache>
                 <c:formatCode>0.00E+00</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>9.1799999999999995E-5</c:v>
+                  <c:v>2.69</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4.8099999999999998E-4</c:v>
+                  <c:v>33.200000000000003</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>6.6600000000000001E-3</c:v>
+                  <c:v>384</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.19600000000000001</c:v>
+                  <c:v>43200</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2.69</c:v>
+                  <c:v>900000</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>33.200000000000003</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>384</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>43200</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>90000</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>90000</c:v>
+                  <c:v>900000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -953,38 +929,33 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$A$26:$A$35</c:f>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>Sheet1!$A$26:$A$35</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>Sheet1!$A$30:$A$35</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>5</c:v>
+                  <c:v>50000</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>50</c:v>
+                  <c:v>500000</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>500</c:v>
+                  <c:v>5000000</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>5000</c:v>
+                  <c:v>50000000</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>50000</c:v>
+                  <c:v>500000000</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>500000</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>5000000</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>50000000</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>500000000</c:v>
-                </c:pt>
-                <c:pt idx="9">
                   <c:v>5000000000</c:v>
                 </c:pt>
               </c:numCache>
@@ -992,39 +963,34 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$G$26:$G$35</c:f>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>Sheet1!$G$26:$G$35</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>Sheet1!$G$30:$G$35</c:f>
               <c:numCache>
                 <c:formatCode>0.00E+00</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>4.1499999999999999E-5</c:v>
+                  <c:v>2.0299999999999998</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3.9899999999999999E-4</c:v>
+                  <c:v>26.6</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>6.8399999999999997E-3</c:v>
+                  <c:v>320</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.159</c:v>
+                  <c:v>3400</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2.0299999999999998</c:v>
+                  <c:v>38800</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>26.6</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>320</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>3400</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>38800</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>90000</c:v>
+                  <c:v>900000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1067,38 +1033,33 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$A$26:$A$35</c:f>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>Sheet1!$A$26:$A$35</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>Sheet1!$A$30:$A$35</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>5</c:v>
+                  <c:v>50000</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>50</c:v>
+                  <c:v>500000</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>500</c:v>
+                  <c:v>5000000</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>5000</c:v>
+                  <c:v>50000000</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>50000</c:v>
+                  <c:v>500000000</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>500000</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>5000000</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>50000000</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>500000000</c:v>
-                </c:pt>
-                <c:pt idx="9">
                   <c:v>5000000000</c:v>
                 </c:pt>
               </c:numCache>
@@ -1106,39 +1067,34 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$H$26:$H$35</c:f>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>Sheet1!$H$26:$H$35</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>Sheet1!$H$30:$H$35</c:f>
               <c:numCache>
                 <c:formatCode>0.00E+00</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>1.37E-4</c:v>
+                  <c:v>0.97799999999999998</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3.59E-4</c:v>
+                  <c:v>12.8</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4.3899999999999998E-3</c:v>
+                  <c:v>138</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>6.3899999999999998E-2</c:v>
+                  <c:v>1500</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.97799999999999998</c:v>
+                  <c:v>19400</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>12.8</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>138</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>1500</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>19400</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>90000</c:v>
+                  <c:v>900000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1147,6 +1103,298 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000007-03AA-4974-ABC9-A5BFD4BD316B}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="8"/>
+          <c:order val="8"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$I$25</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>MT_merge</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent5">
+                  <a:lumMod val="80000"/>
+                  <a:lumOff val="20000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strLit>
+              <c:ptCount val="6"/>
+              <c:pt idx="0">
+                <c:v>50000</c:v>
+              </c:pt>
+              <c:pt idx="1">
+                <c:v>500000</c:v>
+              </c:pt>
+              <c:pt idx="2">
+                <c:v>5000000</c:v>
+              </c:pt>
+              <c:pt idx="3">
+                <c:v>50000000</c:v>
+              </c:pt>
+              <c:pt idx="4">
+                <c:v>500000000</c:v>
+              </c:pt>
+              <c:pt idx="5">
+                <c:v>5000000000</c:v>
+              </c:pt>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:autoCat val="1"/>
+                </c:ext>
+              </c:extLst>
+            </c:strLit>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>Sheet1!$I$26:$I$35</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>Sheet1!$I$30:$I$35</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>1.19</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>8.4499999999999993</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>79.41</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>740</c:v>
+                </c:pt>
+                <c:pt idx="4" formatCode="0.00E+00">
+                  <c:v>8156</c:v>
+                </c:pt>
+                <c:pt idx="5" formatCode="0.00E+00">
+                  <c:v>900000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-DBC9-427B-8674-5EB8C20E56B7}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="9"/>
+          <c:order val="9"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$J$25</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>MT_quick</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="80000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strLit>
+              <c:ptCount val="6"/>
+              <c:pt idx="0">
+                <c:v>50000</c:v>
+              </c:pt>
+              <c:pt idx="1">
+                <c:v>500000</c:v>
+              </c:pt>
+              <c:pt idx="2">
+                <c:v>5000000</c:v>
+              </c:pt>
+              <c:pt idx="3">
+                <c:v>50000000</c:v>
+              </c:pt>
+              <c:pt idx="4">
+                <c:v>500000000</c:v>
+              </c:pt>
+              <c:pt idx="5">
+                <c:v>5000000000</c:v>
+              </c:pt>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:autoCat val="1"/>
+                </c:ext>
+              </c:extLst>
+            </c:strLit>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>Sheet1!$J$26:$J$35</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>Sheet1!$J$30:$J$35</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0.99</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>8.4499999999999993</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>104</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1109</c:v>
+                </c:pt>
+                <c:pt idx="4" formatCode="0.00E+00">
+                  <c:v>10224</c:v>
+                </c:pt>
+                <c:pt idx="5" formatCode="0.00E+00">
+                  <c:v>900000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-DBC9-427B-8674-5EB8C20E56B7}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="10"/>
+          <c:order val="10"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$K$25</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>MT_radix</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3">
+                  <a:lumMod val="80000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strLit>
+              <c:ptCount val="6"/>
+              <c:pt idx="0">
+                <c:v>50000</c:v>
+              </c:pt>
+              <c:pt idx="1">
+                <c:v>500000</c:v>
+              </c:pt>
+              <c:pt idx="2">
+                <c:v>5000000</c:v>
+              </c:pt>
+              <c:pt idx="3">
+                <c:v>50000000</c:v>
+              </c:pt>
+              <c:pt idx="4">
+                <c:v>500000000</c:v>
+              </c:pt>
+              <c:pt idx="5">
+                <c:v>5000000000</c:v>
+              </c:pt>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:autoCat val="1"/>
+                </c:ext>
+              </c:extLst>
+            </c:strLit>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>Sheet1!$K$26:$K$35</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>Sheet1!$K$30:$K$35</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>4.3600000000000003</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5.67</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>12.9</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>119</c:v>
+                </c:pt>
+                <c:pt idx="4" formatCode="0.00E+00">
+                  <c:v>981</c:v>
+                </c:pt>
+                <c:pt idx="5" formatCode="0.00E+00">
+                  <c:v>658669</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-DBC9-427B-8674-5EB8C20E56B7}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1200,42 +1448,33 @@
                   <c:numRef>
                     <c:extLst>
                       <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:fullRef>
+                          <c15:sqref>Sheet1!$A$26:$A$35</c15:sqref>
+                        </c15:fullRef>
                         <c15:formulaRef>
-                          <c15:sqref>Sheet1!$A$26:$A$35</c15:sqref>
+                          <c15:sqref>Sheet1!$A$30:$A$35</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
                     <c:numCache>
                       <c:formatCode>General</c:formatCode>
-                      <c:ptCount val="10"/>
+                      <c:ptCount val="6"/>
                       <c:pt idx="0">
-                        <c:v>5</c:v>
+                        <c:v>50000</c:v>
                       </c:pt>
                       <c:pt idx="1">
-                        <c:v>50</c:v>
+                        <c:v>500000</c:v>
                       </c:pt>
                       <c:pt idx="2">
-                        <c:v>500</c:v>
+                        <c:v>5000000</c:v>
                       </c:pt>
                       <c:pt idx="3">
-                        <c:v>5000</c:v>
+                        <c:v>50000000</c:v>
                       </c:pt>
                       <c:pt idx="4">
-                        <c:v>50000</c:v>
+                        <c:v>500000000</c:v>
                       </c:pt>
                       <c:pt idx="5">
-                        <c:v>500000</c:v>
-                      </c:pt>
-                      <c:pt idx="6">
-                        <c:v>5000000</c:v>
-                      </c:pt>
-                      <c:pt idx="7">
-                        <c:v>50000000</c:v>
-                      </c:pt>
-                      <c:pt idx="8">
-                        <c:v>500000000</c:v>
-                      </c:pt>
-                      <c:pt idx="9">
                         <c:v>5000000000</c:v>
                       </c:pt>
                     </c:numCache>
@@ -1245,42 +1484,33 @@
                   <c:numRef>
                     <c:extLst>
                       <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:fullRef>
+                          <c15:sqref>Sheet1!$A$26:$A$35</c15:sqref>
+                        </c15:fullRef>
                         <c15:formulaRef>
-                          <c15:sqref>Sheet1!$A$26:$A$35</c15:sqref>
+                          <c15:sqref>Sheet1!$A$30:$A$35</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
                     <c:numCache>
                       <c:formatCode>General</c:formatCode>
-                      <c:ptCount val="10"/>
+                      <c:ptCount val="6"/>
                       <c:pt idx="0">
-                        <c:v>5</c:v>
+                        <c:v>50000</c:v>
                       </c:pt>
                       <c:pt idx="1">
-                        <c:v>50</c:v>
+                        <c:v>500000</c:v>
                       </c:pt>
                       <c:pt idx="2">
-                        <c:v>500</c:v>
+                        <c:v>5000000</c:v>
                       </c:pt>
                       <c:pt idx="3">
-                        <c:v>5000</c:v>
+                        <c:v>50000000</c:v>
                       </c:pt>
                       <c:pt idx="4">
-                        <c:v>50000</c:v>
+                        <c:v>500000000</c:v>
                       </c:pt>
                       <c:pt idx="5">
-                        <c:v>500000</c:v>
-                      </c:pt>
-                      <c:pt idx="6">
-                        <c:v>5000000</c:v>
-                      </c:pt>
-                      <c:pt idx="7">
-                        <c:v>50000000</c:v>
-                      </c:pt>
-                      <c:pt idx="8">
-                        <c:v>500000000</c:v>
-                      </c:pt>
-                      <c:pt idx="9">
                         <c:v>5000000000</c:v>
                       </c:pt>
                     </c:numCache>
@@ -1342,7 +1572,7 @@
           </a:p>
         </c:txPr>
         <c:crossAx val="1946842800"/>
-        <c:crosses val="autoZero"/>
+        <c:crossesAt val="0"/>
         <c:auto val="0"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
@@ -1351,9 +1581,9 @@
       <c:valAx>
         <c:axId val="1946842800"/>
         <c:scaling>
-          <c:logBase val="10"/>
           <c:orientation val="minMax"/>
-          <c:max val="8000"/>
+          <c:max val="800000"/>
+          <c:min val="0"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -1405,6 +1635,7 @@
         <c:crossAx val="1946843760"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
+        <c:majorUnit val="50000"/>
       </c:valAx>
       <c:spPr>
         <a:noFill/>
@@ -2049,13 +2280,13 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>381006</xdr:colOff>
       <xdr:row>36</xdr:row>
-      <xdr:rowOff>49530</xdr:rowOff>
+      <xdr:rowOff>57150</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>259080</xdr:colOff>
-      <xdr:row>51</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>586740</xdr:colOff>
+      <xdr:row>63</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2399,717 +2630,804 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<ns0:worksheet xmlns:ns0="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:ns1="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:ns2="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:ns3="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:ns4="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ns1:Ignorable="x14ac xr xr2 xr3" ns2:uid="{CAB68099-47F2-4882-A145-C336AB021326}">
-  <ns0:dimension ref="A1:K35"/>
-  <ns0:sheetViews>
-    <ns0:sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <ns0:pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <ns0:selection pane="topRight" activeCell="H21" sqref="H21"/>
-    </ns0:sheetView>
-  </ns0:sheetViews>
-  <ns0:sheetFormatPr defaultRowHeight="14.4" ns3:dyDescent="0.3"/>
-  <ns0:cols>
-    <ns0:col min="1" max="1" width="22.21875" customWidth="1"/>
-    <ns0:col min="10" max="10" width="9.6640625" bestFit="1" customWidth="1"/>
-    <ns0:col min="11" max="11" width="10.6640625" bestFit="1" customWidth="1"/>
-  </ns0:cols>
-  <ns0:sheetData>
-    <ns0:row r="1" spans="1:11" ns3:dyDescent="0.3">
-      <ns0:c r="A1" s="8" t="s">
-        <ns0:v>16</ns0:v>
-      </ns0:c>
-    </ns0:row>
-    <ns0:row r="2" spans="1:11" ns3:dyDescent="0.3">
-      <ns0:c r="A2" s="1" t="s">
-        <ns0:v>8</ns0:v>
-      </ns0:c>
-    </ns0:row>
-    <ns0:row r="3" spans="1:11" ns3:dyDescent="0.3">
-      <ns0:c r="A3" s="2" t="s">
-        <ns0:v>0</ns0:v>
-      </ns0:c>
-      <ns0:c r="B3" s="23">
-        <ns0:v>5</ns0:v>
-      </ns0:c>
-      <ns0:c r="C3" s="23">
-        <ns0:v>50</ns0:v>
-      </ns0:c>
-      <ns0:c r="D3" s="23">
-        <ns0:v>500</ns0:v>
-      </ns0:c>
-      <ns0:c r="E3" s="23" t="s">
-        <ns0:v>15</ns0:v>
-      </ns0:c>
-      <ns0:c r="F3" s="23" t="s">
-        <ns0:v>14</ns0:v>
-      </ns0:c>
-      <ns0:c r="G3" s="23" t="s">
-        <ns0:v>13</ns0:v>
-      </ns0:c>
-      <ns0:c r="H3" s="23" t="s">
-        <ns0:v>12</ns0:v>
-      </ns0:c>
-      <ns0:c r="I3" s="23" t="s">
-        <ns0:v>11</ns0:v>
-      </ns0:c>
-      <ns0:c r="J3" s="23" t="s">
-        <ns0:v>10</ns0:v>
-      </ns0:c>
-      <ns0:c r="K3" s="23" t="s">
-        <ns0:v>9</ns0:v>
-      </ns0:c>
-    </ns0:row>
-    <ns0:row r="4" spans="1:11" ns3:dyDescent="0.3">
-      <ns0:c r="A4" s="3" t="s">
-        <ns0:v>1</ns0:v>
-      </ns0:c>
-      <ns0:c r="B4" s="9">
-        <ns0:v>3.8600000000000003E-5</ns0:v>
-      </ns0:c>
-      <ns0:c r="C4" s="9">
-        <ns0:v>7.7899999999999996E-4</ns0:v>
-      </ns0:c>
-      <ns0:c r="D4" s="9">
-        <ns0:v>1.38E-2</ns0:v>
-      </ns0:c>
-      <ns0:c r="E4" s="9">
-        <ns0:v>0.96</ns0:v>
-      </ns0:c>
-      <ns0:c r="F4" s="9">
-        <ns0:v>86.7</ns0:v>
-      </ns0:c>
-      <ns0:c r="G4" s="9">
-        <ns0:v>10000</ns0:v>
-      </ns0:c>
-      <ns0:c r="H4" s="10" t="s">
-        <ns0:v>18</ns0:v>
-      </ns0:c>
-      <ns0:c r="I4" s="10" t="s">
-        <ns0:v>18</ns0:v>
-      </ns0:c>
-      <ns0:c r="J4" s="10" t="s">
-        <ns0:v>18</ns0:v>
-      </ns0:c>
-      <ns0:c r="K4" s="10" t="s">
-        <ns0:v>18</ns0:v>
-      </ns0:c>
-    </ns0:row>
-    <ns0:row r="5" spans="1:11" ns3:dyDescent="0.3">
-      <ns0:c r="A5" s="4" t="s">
-        <ns0:v>2</ns0:v>
-      </ns0:c>
-      <ns0:c r="B5" s="11">
-        <ns0:v>4.4400000000000002E-5</ns0:v>
-      </ns0:c>
-      <ns0:c r="C5" s="11">
-        <ns0:v>6.3000000000000003E-4</ns0:v>
-      </ns0:c>
-      <ns0:c r="D5" s="11">
-        <ns0:v>4.0800000000000003E-2</ns0:v>
-      </ns0:c>
-      <ns0:c r="E5" s="11">
-        <ns0:v>2.76</ns0:v>
-      </ns0:c>
-      <ns0:c r="F5" s="11">
-        <ns0:v>264</ns0:v>
-      </ns0:c>
-      <ns0:c r="G5" s="11">
-        <ns0:v>25400</ns0:v>
-      </ns0:c>
-      <ns0:c r="H5" s="12" t="s">
-        <ns0:v>18</ns0:v>
-      </ns0:c>
-      <ns0:c r="I5" s="12" t="s">
-        <ns0:v>18</ns0:v>
-      </ns0:c>
-      <ns0:c r="J5" s="12" t="s">
-        <ns0:v>18</ns0:v>
-      </ns0:c>
-      <ns0:c r="K5" s="12" t="s">
-        <ns0:v>18</ns0:v>
-      </ns0:c>
-    </ns0:row>
-    <ns0:row r="6" spans="1:11" ns3:dyDescent="0.3">
-      <ns0:c r="A6" s="5" t="s">
-        <ns0:v>3</ns0:v>
-      </ns0:c>
-      <ns0:c r="B6" s="13">
-        <ns0:v>4.4100000000000001E-5</ns0:v>
-      </ns0:c>
-      <ns0:c r="C6" s="13">
-        <ns0:v>4.3399999999999998E-4</ns0:v>
-      </ns0:c>
-      <ns0:c r="D6" s="13">
-        <ns0:v>6.9800000000000001E-3</ns0:v>
-      </ns0:c>
-      <ns0:c r="E6" s="13">
-        <ns0:v>0.25600000000000001</ns0:v>
-      </ns0:c>
-      <ns0:c r="F6" s="13">
-        <ns0:v>3.7</ns0:v>
-      </ns0:c>
-      <ns0:c r="G6" s="13">
-        <ns0:v>49.3</ns0:v>
-      </ns0:c>
-      <ns0:c r="H6" s="13">
-        <ns0:v>626</ns0:v>
-      </ns0:c>
-      <ns0:c r="I6" s="13">
-        <ns0:v>82800</ns0:v>
-      </ns0:c>
-      <ns0:c r="J6" s="14" t="s">
-        <ns0:v>17</ns0:v>
-      </ns0:c>
-      <ns0:c r="K6" s="14" t="s">
-        <ns0:v>17</ns0:v>
-      </ns0:c>
-    </ns0:row>
-    <ns0:row r="7" spans="1:11" ns3:dyDescent="0.3">
-      <ns0:c r="A7" s="1" t="s">
-        <ns0:v>4</ns0:v>
-      </ns0:c>
-      <ns0:c r="B7" s="15">
-        <ns0:v>3.0599999999999998E-5</ns0:v>
-      </ns0:c>
-      <ns0:c r="C7" s="15">
-        <ns0:v>4.4099999999999999E-4</ns0:v>
-      </ns0:c>
-      <ns0:c r="D7" s="15">
-        <ns0:v>5.3E-3</ns0:v>
-      </ns0:c>
-      <ns0:c r="E7" s="15">
-        <ns0:v>0.121</ns0:v>
-      </ns0:c>
-      <ns0:c r="F7" s="15">
-        <ns0:v>1.83</ns0:v>
-      </ns0:c>
-      <ns0:c r="G7" s="15">
-        <ns0:v>9.84</ns0:v>
-      </ns0:c>
-      <ns0:c r="H7" s="15">
-        <ns0:v>604</ns0:v>
-      </ns0:c>
-      <ns0:c r="I7" s="15">
-        <ns0:v>30800</ns0:v>
-      </ns0:c>
-      <ns0:c r="J7" s="16" t="s">
-        <ns0:v>17</ns0:v>
-      </ns0:c>
-      <ns0:c r="K7" s="16" t="s">
-        <ns0:v>17</ns0:v>
-      </ns0:c>
-    </ns0:row>
-    <ns0:row r="8" spans="1:11" ns3:dyDescent="0.3">
-      <ns0:c r="A8" s="6" t="s">
-        <ns0:v>5</ns0:v>
-      </ns0:c>
-      <ns0:c r="B8" s="17">
-        <ns0:v>9.1799999999999995E-5</ns0:v>
-      </ns0:c>
-      <ns0:c r="C8" s="17">
-        <ns0:v>4.8099999999999998E-4</ns0:v>
-      </ns0:c>
-      <ns0:c r="D8" s="17">
-        <ns0:v>6.6600000000000001E-3</ns0:v>
-      </ns0:c>
-      <ns0:c r="E8" s="17">
-        <ns0:v>0.19600000000000001</ns0:v>
-      </ns0:c>
-      <ns0:c r="F8" s="17">
-        <ns0:v>2.69</ns0:v>
-      </ns0:c>
-      <ns0:c r="G8" s="17">
-        <ns0:v>33.200000000000003</ns0:v>
-      </ns0:c>
-      <ns0:c r="H8" s="17">
-        <ns0:v>384</ns0:v>
-      </ns0:c>
-      <ns0:c r="I8" s="17">
-        <ns0:v>43200</ns0:v>
-      </ns0:c>
-      <ns0:c r="J8" s="18" t="s">
-        <ns0:v>17</ns0:v>
-      </ns0:c>
-      <ns0:c r="K8" s="18">
-        <ns0:v>658669</ns0:v>
-      </ns0:c>
-    </ns0:row>
-    <ns0:row r="9" spans="1:11" ns3:dyDescent="0.3">
-      <ns0:c r="A9" s="7" t="s">
-        <ns0:v>6</ns0:v>
-      </ns0:c>
-      <ns0:c r="B9" s="19">
-        <ns0:v>4.1499999999999999E-5</ns0:v>
-      </ns0:c>
-      <ns0:c r="C9" s="19">
-        <ns0:v>3.9899999999999999E-4</ns0:v>
-      </ns0:c>
-      <ns0:c r="D9" s="19">
-        <ns0:v>6.8399999999999997E-3</ns0:v>
-      </ns0:c>
-      <ns0:c r="E9" s="19">
-        <ns0:v>0.159</ns0:v>
-      </ns0:c>
-      <ns0:c r="F9" s="19">
-        <ns0:v>2.0299999999999998</ns0:v>
-      </ns0:c>
-      <ns0:c r="G9" s="19">
-        <ns0:v>26.6</ns0:v>
-      </ns0:c>
-      <ns0:c r="H9" s="19">
-        <ns0:v>320</ns0:v>
-      </ns0:c>
-      <ns0:c r="I9" s="19">
-        <ns0:v>3400</ns0:v>
-      </ns0:c>
-      <ns0:c r="J9" s="19">
-        <ns0:v>38800</ns0:v>
-      </ns0:c>
-      <ns0:c r="K9" s="20" t="s">
-        <ns0:v>17</ns0:v>
-      </ns0:c>
-    </ns0:row>
-    <ns0:row r="10" spans="1:11" ns3:dyDescent="0.3">
-      <ns0:c r="A10" s="8" t="s">
-        <ns0:v>7</ns0:v>
-      </ns0:c>
-      <ns0:c r="B10" s="21">
-        <ns0:v>1.37E-4</ns0:v>
-      </ns0:c>
-      <ns0:c r="C10" s="21">
-        <ns0:v>3.59E-4</ns0:v>
-      </ns0:c>
-      <ns0:c r="D10" s="21">
-        <ns0:v>4.3899999999999998E-3</ns0:v>
-      </ns0:c>
-      <ns0:c r="E10" s="21">
-        <ns0:v>6.3899999999999998E-2</ns0:v>
-      </ns0:c>
-      <ns0:c r="F10" s="21">
-        <ns0:v>0.97799999999999998</ns0:v>
-      </ns0:c>
-      <ns0:c r="G10" s="21">
-        <ns0:v>12.8</ns0:v>
-      </ns0:c>
-      <ns0:c r="H10" s="21">
-        <ns0:v>138</ns0:v>
-      </ns0:c>
-      <ns0:c r="I10" s="21">
-        <ns0:v>1500</ns0:v>
-      </ns0:c>
-      <ns0:c r="J10" s="21">
-        <ns0:v>19400</ns0:v>
-      </ns0:c>
-      <ns0:c r="K10" s="22" t="s">
-        <ns0:v>17</ns0:v>
-      </ns0:c>
-    </ns0:row>
-    <ns0:row r="25" spans="1:8" ns3:dyDescent="0.3">
-      <ns0:c r="A25" t="s">
-        <ns0:v>19</ns0:v>
-      </ns0:c>
-      <ns0:c r="B25" t="s">
-        <ns0:v>20</ns0:v>
-      </ns0:c>
-      <ns0:c r="C25" t="s">
-        <ns0:v>21</ns0:v>
-      </ns0:c>
-      <ns0:c r="D25" t="s">
-        <ns0:v>22</ns0:v>
-      </ns0:c>
-      <ns0:c r="E25" t="s">
-        <ns0:v>23</ns0:v>
-      </ns0:c>
-      <ns0:c r="F25" t="s">
-        <ns0:v>24</ns0:v>
-      </ns0:c>
-      <ns0:c r="G25" t="s">
-        <ns0:v>25</ns0:v>
-      </ns0:c>
-      <ns0:c r="H25" t="s">
-        <ns0:v>26</ns0:v>
-      </ns0:c>
-    </ns0:row>
-    <ns0:row r="26" spans="1:8" ns3:dyDescent="0.3">
-      <ns0:c r="A26">
-        <ns0:v>5</ns0:v>
-      </ns0:c>
-      <ns0:c r="B26" s="9">
-        <ns0:v>3.8600000000000003E-5</ns0:v>
-      </ns0:c>
-      <ns0:c r="C26" s="11">
-        <ns0:v>4.4400000000000002E-5</ns0:v>
-      </ns0:c>
-      <ns0:c r="D26" s="13">
-        <ns0:v>4.4100000000000001E-5</ns0:v>
-      </ns0:c>
-      <ns0:c r="E26" s="15">
-        <ns0:v>3.0599999999999998E-5</ns0:v>
-      </ns0:c>
-      <ns0:c r="F26" s="17">
-        <ns0:v>9.1799999999999995E-5</ns0:v>
-      </ns0:c>
-      <ns0:c r="G26" s="19">
-        <ns0:v>4.1499999999999999E-5</ns0:v>
-      </ns0:c>
-      <ns0:c r="H26" s="21">
-        <ns0:v>1.37E-4</ns0:v>
-      </ns0:c>
-    </ns0:row>
-    <ns0:row r="27" spans="1:8" ns3:dyDescent="0.3">
-      <ns0:c r="A27">
-        <ns0:v>50</ns0:v>
-      </ns0:c>
-      <ns0:c r="B27" s="9">
-        <ns0:v>7.7899999999999996E-4</ns0:v>
-      </ns0:c>
-      <ns0:c r="C27" s="11">
-        <ns0:v>6.3000000000000003E-4</ns0:v>
-      </ns0:c>
-      <ns0:c r="D27" s="13">
-        <ns0:v>4.3399999999999998E-4</ns0:v>
-      </ns0:c>
-      <ns0:c r="E27" s="15">
-        <ns0:v>4.4099999999999999E-4</ns0:v>
-      </ns0:c>
-      <ns0:c r="F27" s="17">
-        <ns0:v>4.8099999999999998E-4</ns0:v>
-      </ns0:c>
-      <ns0:c r="G27" s="19">
-        <ns0:v>3.9899999999999999E-4</ns0:v>
-      </ns0:c>
-      <ns0:c r="H27" s="21">
-        <ns0:v>3.59E-4</ns0:v>
-      </ns0:c>
-    </ns0:row>
-    <ns0:row r="28" spans="1:8" ns3:dyDescent="0.3">
-      <ns0:c r="A28">
-        <ns0:v>500</ns0:v>
-      </ns0:c>
-      <ns0:c r="B28" s="9">
-        <ns0:v>1.38E-2</ns0:v>
-      </ns0:c>
-      <ns0:c r="C28" s="11">
-        <ns0:v>4.0800000000000003E-2</ns0:v>
-      </ns0:c>
-      <ns0:c r="D28" s="13">
-        <ns0:v>6.9800000000000001E-3</ns0:v>
-      </ns0:c>
-      <ns0:c r="E28" s="15">
-        <ns0:v>5.3E-3</ns0:v>
-      </ns0:c>
-      <ns0:c r="F28" s="17">
-        <ns0:v>6.6600000000000001E-3</ns0:v>
-      </ns0:c>
-      <ns0:c r="G28" s="19">
-        <ns0:v>6.8399999999999997E-3</ns0:v>
-      </ns0:c>
-      <ns0:c r="H28" s="21">
-        <ns0:v>4.3899999999999998E-3</ns0:v>
-      </ns0:c>
-    </ns0:row>
-    <ns0:row r="29" spans="1:8" ns3:dyDescent="0.3">
-      <ns0:c r="A29">
-        <ns0:v>5000</ns0:v>
-      </ns0:c>
-      <ns0:c r="B29" s="9">
-        <ns0:v>0.96</ns0:v>
-      </ns0:c>
-      <ns0:c r="C29" s="11">
-        <ns0:v>2.76</ns0:v>
-      </ns0:c>
-      <ns0:c r="D29" s="13">
-        <ns0:v>0.25600000000000001</ns0:v>
-      </ns0:c>
-      <ns0:c r="E29" s="15">
-        <ns0:v>0.121</ns0:v>
-      </ns0:c>
-      <ns0:c r="F29" s="17">
-        <ns0:v>0.19600000000000001</ns0:v>
-      </ns0:c>
-      <ns0:c r="G29" s="19">
-        <ns0:v>0.159</ns0:v>
-      </ns0:c>
-      <ns0:c r="H29" s="21">
-        <ns0:v>6.3899999999999998E-2</ns0:v>
-      </ns0:c>
-    </ns0:row>
-    <ns0:row r="30" spans="1:8" ns3:dyDescent="0.3">
-      <ns0:c r="A30">
-        <ns0:v>50000</ns0:v>
-      </ns0:c>
-      <ns0:c r="B30" s="9">
-        <ns0:v>86.7</ns0:v>
-      </ns0:c>
-      <ns0:c r="C30" s="11">
-        <ns0:v>264</ns0:v>
-      </ns0:c>
-      <ns0:c r="D30" s="13">
-        <ns0:v>3.7</ns0:v>
-      </ns0:c>
-      <ns0:c r="E30" s="15">
-        <ns0:v>1.83</ns0:v>
-      </ns0:c>
-      <ns0:c r="F30" s="17">
-        <ns0:v>2.69</ns0:v>
-      </ns0:c>
-      <ns0:c r="G30" s="19">
-        <ns0:v>2.0299999999999998</ns0:v>
-      </ns0:c>
-      <ns0:c r="H30" s="21">
-        <ns0:v>0.97799999999999998</ns0:v>
-      </ns0:c>
-    </ns0:row>
-    <ns0:row r="31" spans="1:8" ns3:dyDescent="0.3">
-      <ns0:c r="A31">
-        <ns0:v>500000</ns0:v>
-      </ns0:c>
-      <ns0:c r="B31" s="9">
-        <ns0:v>10000</ns0:v>
-      </ns0:c>
-      <ns0:c r="C31" s="11">
-        <ns0:v>25400</ns0:v>
-      </ns0:c>
-      <ns0:c r="D31" s="13">
-        <ns0:v>49.3</ns0:v>
-      </ns0:c>
-      <ns0:c r="E31" s="15">
-        <ns0:v>9.84</ns0:v>
-      </ns0:c>
-      <ns0:c r="F31" s="17">
-        <ns0:v>33.200000000000003</ns0:v>
-      </ns0:c>
-      <ns0:c r="G31" s="19">
-        <ns0:v>26.6</ns0:v>
-      </ns0:c>
-      <ns0:c r="H31" s="21">
-        <ns0:v>12.8</ns0:v>
-      </ns0:c>
-    </ns0:row>
-    <ns0:row r="32" spans="1:8" ns3:dyDescent="0.3">
-      <ns0:c r="A32">
-        <ns0:v>5000000</ns0:v>
-      </ns0:c>
-      <ns0:c r="B32" s="24">
-        <ns0:v>90000</ns0:v>
-      </ns0:c>
-      <ns0:c r="C32" s="24">
-        <ns0:v>90000</ns0:v>
-      </ns0:c>
-      <ns0:c r="D32" s="13">
-        <ns0:v>626</ns0:v>
-      </ns0:c>
-      <ns0:c r="E32" s="15">
-        <ns0:v>604</ns0:v>
-      </ns0:c>
-      <ns0:c r="F32" s="17">
-        <ns0:v>384</ns0:v>
-      </ns0:c>
-      <ns0:c r="G32" s="19">
-        <ns0:v>320</ns0:v>
-      </ns0:c>
-      <ns0:c r="H32" s="21">
-        <ns0:v>138</ns0:v>
-      </ns0:c>
-    </ns0:row>
-    <ns0:row r="33" spans="1:8" ns3:dyDescent="0.3">
-      <ns0:c r="A33">
-        <ns0:v>50000000</ns0:v>
-      </ns0:c>
-      <ns0:c r="B33" s="24">
-        <ns0:v>90000</ns0:v>
-      </ns0:c>
-      <ns0:c r="C33" s="24">
-        <ns0:v>90000</ns0:v>
-      </ns0:c>
-      <ns0:c r="D33" s="13">
-        <ns0:v>82800</ns0:v>
-      </ns0:c>
-      <ns0:c r="E33" s="15">
-        <ns0:v>30800</ns0:v>
-      </ns0:c>
-      <ns0:c r="F33" s="17">
-        <ns0:v>43200</ns0:v>
-      </ns0:c>
-      <ns0:c r="G33" s="19">
-        <ns0:v>3400</ns0:v>
-      </ns0:c>
-      <ns0:c r="H33" s="21">
-        <ns0:v>1500</ns0:v>
-      </ns0:c>
-    </ns0:row>
-    <ns0:row r="34" spans="1:8" ns3:dyDescent="0.3">
-      <ns0:c r="A34">
-        <ns0:v>500000000</ns0:v>
-      </ns0:c>
-      <ns0:c r="B34" s="24">
-        <ns0:v>90000</ns0:v>
-      </ns0:c>
-      <ns0:c r="C34" s="24">
-        <ns0:v>90000</ns0:v>
-      </ns0:c>
-      <ns0:c r="D34" s="24">
-        <ns0:v>90000</ns0:v>
-      </ns0:c>
-      <ns0:c r="E34" s="24">
-        <ns0:v>90000</ns0:v>
-      </ns0:c>
-      <ns0:c r="F34" s="24">
-        <ns0:v>90000</ns0:v>
-      </ns0:c>
-      <ns0:c r="G34" s="19">
-        <ns0:v>38800</ns0:v>
-      </ns0:c>
-      <ns0:c r="H34" s="21">
-        <ns0:v>19400</ns0:v>
-      </ns0:c>
-    </ns0:row>
-    <ns0:row r="35" spans="1:8" ns3:dyDescent="0.3">
-      <ns0:c r="A35">
-        <ns0:v>5000000000</ns0:v>
-      </ns0:c>
-      <ns0:c r="B35" s="24">
-        <ns0:v>90000</ns0:v>
-      </ns0:c>
-      <ns0:c r="C35" s="24">
-        <ns0:v>90000</ns0:v>
-      </ns0:c>
-      <ns0:c r="D35" s="24">
-        <ns0:v>90000</ns0:v>
-      </ns0:c>
-      <ns0:c r="E35" s="24">
-        <ns0:v>90000</ns0:v>
-      </ns0:c>
-      <ns0:c r="F35" s="24">
-        <ns0:v>90000</ns0:v>
-      </ns0:c>
-      <ns0:c r="G35" s="24">
-        <ns0:v>90000</ns0:v>
-      </ns0:c>
-      <ns0:c r="H35" s="24">
-        <ns0:v>90000</ns0:v>
-      </ns0:c>
-    </ns0:row>
-    <ns0:row r="8">
-      <ns0:c r="A8" t="inlineStr">
-        <ns0:is>
-          <ns0:t>MT Radix</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="B8">
-        <ns0:v>3.37439</ns0:v>
-      </ns0:c>
-      <ns0:c r="C8">
-        <ns0:v>4.68975</ns0:v>
-      </ns0:c>
-      <ns0:c r="D8">
-        <ns0:v>3.582</ns0:v>
-      </ns0:c>
-      <ns0:c r="E8">
-        <ns0:v>3.51248</ns0:v>
-      </ns0:c>
-      <ns0:c r="F8">
-        <ns0:v>4.3622</ns0:v>
-      </ns0:c>
-      <ns0:c r="G8">
-        <ns0:v>5.66774</ns0:v>
-      </ns0:c>
-      <ns0:c r="H8">
-        <ns0:v>12.8233</ns0:v>
-      </ns0:c>
-      <ns0:c r="I8">
-        <ns0:v>118.616</ns0:v>
-      </ns0:c>
-      <ns0:c r="J8">
-        <ns0:v>980.61</ns0:v>
-      </ns0:c>
-      <ns0:c r="K8" t="inlineStr">
-        <ns0:is>
-          <ns0:t>TBD</ns0:t>
-        </ns0:is>
-      </ns0:c>
-    </ns0:row>
-    <ns0:row r="9">
-      <ns0:c r="A9" t="inlineStr">
-        <ns0:is>
-          <ns0:t>MT Merge</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="B9">
-        <ns0:v>0.0044881</ns0:v>
-      </ns0:c>
-      <ns0:c r="C9">
-        <ns0:v>0.0041136</ns0:v>
-      </ns0:c>
-      <ns0:c r="D9">
-        <ns0:v>0.0086389</ns0:v>
-      </ns0:c>
-      <ns0:c r="E9">
-        <ns0:v>0.173374</ns0:v>
-      </ns0:c>
-      <ns0:c r="F9">
-        <ns0:v>1.1888</ns0:v>
-      </ns0:c>
-      <ns0:c r="G9">
-        <ns0:v>8.44872</ns0:v>
-      </ns0:c>
-      <ns0:c r="H9">
-        <ns0:v>79.4147</ns0:v>
-      </ns0:c>
-      <ns0:c r="I9">
-        <ns0:v>740</ns0:v>
-      </ns0:c>
-      <ns0:c r="J9">
-        <ns0:v>8156.47</ns0:v>
-      </ns0:c>
-      <ns0:c r="K9" t="inlineStr">
-        <ns0:is>
-          <ns0:t>TBD</ns0:t>
-        </ns0:is>
-      </ns0:c>
-    </ns0:row>
-    <ns0:row r="10">
-      <ns0:c r="A10" t="inlineStr">
-        <ns0:is>
-          <ns0:t>MT Quick</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="B10">
-        <ns0:v>0.0038483</ns0:v>
-      </ns0:c>
-      <ns0:c r="C10">
-        <ns0:v>0.00663</ns0:v>
-      </ns0:c>
-      <ns0:c r="D10">
-        <ns0:v>0.0090138</ns0:v>
-      </ns0:c>
-      <ns0:c r="E10">
-        <ns0:v>0.148835</ns0:v>
-      </ns0:c>
-      <ns0:c r="F10">
-        <ns0:v>0.990992</ns0:v>
-      </ns0:c>
-      <ns0:c r="G10">
-        <ns0:v>8.44602</ns0:v>
-      </ns0:c>
-      <ns0:c r="H10">
-        <ns0:v>103.908</ns0:v>
-      </ns0:c>
-      <ns0:c r="I10">
-        <ns0:v>1108.83</ns0:v>
-      </ns0:c>
-      <ns0:c r="J10">
-        <ns0:v>10224</ns0:v>
-      </ns0:c>
-      <ns0:c r="K10" t="inlineStr">
-        <ns0:is>
-          <ns0:t>TBD</ns0:t>
-        </ns0:is>
-      </ns0:c>
-    </ns0:row>
-  </ns0:sheetData>
-  <ns0:pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <ns0:pageSetup orientation="portrait" verticalDpi="0" ns4:id="rId1"/>
-  <ns0:drawing ns4:id="rId2"/>
-</ns0:worksheet>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CAB68099-47F2-4882-A145-C336AB021326}">
+  <dimension ref="A1:K35"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="R22" sqref="R22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="22.21875" customWidth="1"/>
+    <col min="10" max="10" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A1" s="8" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="23">
+        <v>5</v>
+      </c>
+      <c r="C3" s="23">
+        <v>50</v>
+      </c>
+      <c r="D3" s="23">
+        <v>500</v>
+      </c>
+      <c r="E3" s="23" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3" s="23" t="s">
+        <v>14</v>
+      </c>
+      <c r="G3" s="23" t="s">
+        <v>13</v>
+      </c>
+      <c r="H3" s="23" t="s">
+        <v>12</v>
+      </c>
+      <c r="I3" s="23" t="s">
+        <v>11</v>
+      </c>
+      <c r="J3" s="23" t="s">
+        <v>10</v>
+      </c>
+      <c r="K3" s="23" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A4" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" s="9">
+        <v>3.8600000000000003E-5</v>
+      </c>
+      <c r="C4" s="9">
+        <v>7.7899999999999996E-4</v>
+      </c>
+      <c r="D4" s="9">
+        <v>1.38E-2</v>
+      </c>
+      <c r="E4" s="9">
+        <v>0.96</v>
+      </c>
+      <c r="F4" s="9">
+        <v>86.7</v>
+      </c>
+      <c r="G4" s="9">
+        <v>10000</v>
+      </c>
+      <c r="H4" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="I4" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="J4" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="K4" s="10" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A5" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" s="11">
+        <v>4.4400000000000002E-5</v>
+      </c>
+      <c r="C5" s="11">
+        <v>6.3000000000000003E-4</v>
+      </c>
+      <c r="D5" s="11">
+        <v>4.0800000000000003E-2</v>
+      </c>
+      <c r="E5" s="11">
+        <v>2.76</v>
+      </c>
+      <c r="F5" s="11">
+        <v>264</v>
+      </c>
+      <c r="G5" s="11">
+        <v>25400</v>
+      </c>
+      <c r="H5" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="I5" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="J5" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="K5" s="12" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A6" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" s="13">
+        <v>4.4100000000000001E-5</v>
+      </c>
+      <c r="C6" s="13">
+        <v>4.3399999999999998E-4</v>
+      </c>
+      <c r="D6" s="13">
+        <v>6.9800000000000001E-3</v>
+      </c>
+      <c r="E6" s="13">
+        <v>0.25600000000000001</v>
+      </c>
+      <c r="F6" s="13">
+        <v>3.7</v>
+      </c>
+      <c r="G6" s="13">
+        <v>49.3</v>
+      </c>
+      <c r="H6" s="13">
+        <v>626</v>
+      </c>
+      <c r="I6" s="13">
+        <v>82800</v>
+      </c>
+      <c r="J6" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="K6" s="14" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7" s="15">
+        <v>3.0599999999999998E-5</v>
+      </c>
+      <c r="C7" s="15">
+        <v>4.4099999999999999E-4</v>
+      </c>
+      <c r="D7" s="15">
+        <v>5.3E-3</v>
+      </c>
+      <c r="E7" s="15">
+        <v>0.121</v>
+      </c>
+      <c r="F7" s="15">
+        <v>1.83</v>
+      </c>
+      <c r="G7" s="15">
+        <v>9.84</v>
+      </c>
+      <c r="H7" s="15">
+        <v>604</v>
+      </c>
+      <c r="I7" s="15">
+        <v>30800</v>
+      </c>
+      <c r="J7" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="K7" s="16" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A8" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8" s="17">
+        <v>9.1799999999999995E-5</v>
+      </c>
+      <c r="C8" s="17">
+        <v>4.8099999999999998E-4</v>
+      </c>
+      <c r="D8" s="17">
+        <v>6.6600000000000001E-3</v>
+      </c>
+      <c r="E8" s="17">
+        <v>0.19600000000000001</v>
+      </c>
+      <c r="F8" s="17">
+        <v>2.69</v>
+      </c>
+      <c r="G8" s="17">
+        <v>33.200000000000003</v>
+      </c>
+      <c r="H8" s="17">
+        <v>384</v>
+      </c>
+      <c r="I8" s="17">
+        <v>43200</v>
+      </c>
+      <c r="J8" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="K8" s="18" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A9" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" s="19">
+        <v>4.1499999999999999E-5</v>
+      </c>
+      <c r="C9" s="19">
+        <v>3.9899999999999999E-4</v>
+      </c>
+      <c r="D9" s="19">
+        <v>6.8399999999999997E-3</v>
+      </c>
+      <c r="E9" s="19">
+        <v>0.159</v>
+      </c>
+      <c r="F9" s="19">
+        <v>2.0299999999999998</v>
+      </c>
+      <c r="G9" s="19">
+        <v>26.6</v>
+      </c>
+      <c r="H9" s="19">
+        <v>320</v>
+      </c>
+      <c r="I9" s="19">
+        <v>3400</v>
+      </c>
+      <c r="J9" s="19">
+        <v>38800</v>
+      </c>
+      <c r="K9" s="20" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A10" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B10" s="21">
+        <v>1.37E-4</v>
+      </c>
+      <c r="C10" s="21">
+        <v>3.59E-4</v>
+      </c>
+      <c r="D10" s="21">
+        <v>4.3899999999999998E-3</v>
+      </c>
+      <c r="E10" s="21">
+        <v>6.3899999999999998E-2</v>
+      </c>
+      <c r="F10" s="21">
+        <v>0.97799999999999998</v>
+      </c>
+      <c r="G10" s="21">
+        <v>12.8</v>
+      </c>
+      <c r="H10" s="21">
+        <v>138</v>
+      </c>
+      <c r="I10" s="21">
+        <v>1500</v>
+      </c>
+      <c r="J10" s="21">
+        <v>19400</v>
+      </c>
+      <c r="K10" s="22" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>28</v>
+      </c>
+      <c r="B11">
+        <v>4.4999999999999997E-3</v>
+      </c>
+      <c r="C11">
+        <v>4.1000000000000003E-3</v>
+      </c>
+      <c r="D11">
+        <v>8.6E-3</v>
+      </c>
+      <c r="E11">
+        <v>0.17</v>
+      </c>
+      <c r="F11">
+        <v>1.19</v>
+      </c>
+      <c r="G11">
+        <v>8.4499999999999993</v>
+      </c>
+      <c r="H11">
+        <v>79.41</v>
+      </c>
+      <c r="I11">
+        <v>740</v>
+      </c>
+      <c r="J11">
+        <v>8160</v>
+      </c>
+      <c r="K11" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>27</v>
+      </c>
+      <c r="B12">
+        <v>3.8E-3</v>
+      </c>
+      <c r="C12">
+        <v>6.6E-3</v>
+      </c>
+      <c r="D12">
+        <v>8.9999999999999993E-3</v>
+      </c>
+      <c r="E12">
+        <v>0.15</v>
+      </c>
+      <c r="F12">
+        <v>0.99</v>
+      </c>
+      <c r="G12">
+        <v>8.4499999999999993</v>
+      </c>
+      <c r="H12">
+        <v>104</v>
+      </c>
+      <c r="I12">
+        <v>1109</v>
+      </c>
+      <c r="J12">
+        <v>10200</v>
+      </c>
+      <c r="K12" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>29</v>
+      </c>
+      <c r="B13">
+        <v>3.37</v>
+      </c>
+      <c r="C13">
+        <v>4.6900000000000004</v>
+      </c>
+      <c r="D13">
+        <v>3.58</v>
+      </c>
+      <c r="E13">
+        <v>3.61</v>
+      </c>
+      <c r="F13">
+        <v>4.3600000000000003</v>
+      </c>
+      <c r="G13">
+        <v>5.67</v>
+      </c>
+      <c r="H13">
+        <v>12.9</v>
+      </c>
+      <c r="I13">
+        <v>119</v>
+      </c>
+      <c r="J13">
+        <v>981</v>
+      </c>
+      <c r="K13">
+        <v>659000</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>19</v>
+      </c>
+      <c r="B25" t="s">
+        <v>20</v>
+      </c>
+      <c r="C25" t="s">
+        <v>21</v>
+      </c>
+      <c r="D25" t="s">
+        <v>22</v>
+      </c>
+      <c r="E25" t="s">
+        <v>23</v>
+      </c>
+      <c r="F25" t="s">
+        <v>24</v>
+      </c>
+      <c r="G25" t="s">
+        <v>25</v>
+      </c>
+      <c r="H25" t="s">
+        <v>26</v>
+      </c>
+      <c r="I25" t="s">
+        <v>28</v>
+      </c>
+      <c r="J25" t="s">
+        <v>27</v>
+      </c>
+      <c r="K25" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A26">
+        <v>5</v>
+      </c>
+      <c r="B26" s="9">
+        <v>3.8600000000000003E-5</v>
+      </c>
+      <c r="C26" s="11">
+        <v>4.4400000000000002E-5</v>
+      </c>
+      <c r="D26" s="13">
+        <v>4.4100000000000001E-5</v>
+      </c>
+      <c r="E26" s="15">
+        <v>3.0599999999999998E-5</v>
+      </c>
+      <c r="F26" s="17">
+        <v>9.1799999999999995E-5</v>
+      </c>
+      <c r="G26" s="19">
+        <v>4.1499999999999999E-5</v>
+      </c>
+      <c r="H26" s="21">
+        <v>1.37E-4</v>
+      </c>
+      <c r="I26" s="2">
+        <v>4.4999999999999997E-3</v>
+      </c>
+      <c r="J26" s="26">
+        <v>3.8E-3</v>
+      </c>
+      <c r="K26" s="28">
+        <v>3.37</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A27">
+        <v>50</v>
+      </c>
+      <c r="B27" s="9">
+        <v>7.7899999999999996E-4</v>
+      </c>
+      <c r="C27" s="11">
+        <v>6.3000000000000003E-4</v>
+      </c>
+      <c r="D27" s="13">
+        <v>4.3399999999999998E-4</v>
+      </c>
+      <c r="E27" s="15">
+        <v>4.4099999999999999E-4</v>
+      </c>
+      <c r="F27" s="17">
+        <v>4.8099999999999998E-4</v>
+      </c>
+      <c r="G27" s="19">
+        <v>3.9899999999999999E-4</v>
+      </c>
+      <c r="H27" s="21">
+        <v>3.59E-4</v>
+      </c>
+      <c r="I27" s="2">
+        <v>4.1000000000000003E-3</v>
+      </c>
+      <c r="J27" s="26">
+        <v>6.6E-3</v>
+      </c>
+      <c r="K27" s="28">
+        <v>4.6900000000000004</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A28">
+        <v>500</v>
+      </c>
+      <c r="B28" s="9">
+        <v>1.38E-2</v>
+      </c>
+      <c r="C28" s="11">
+        <v>4.0800000000000003E-2</v>
+      </c>
+      <c r="D28" s="13">
+        <v>6.9800000000000001E-3</v>
+      </c>
+      <c r="E28" s="15">
+        <v>5.3E-3</v>
+      </c>
+      <c r="F28" s="17">
+        <v>6.6600000000000001E-3</v>
+      </c>
+      <c r="G28" s="19">
+        <v>6.8399999999999997E-3</v>
+      </c>
+      <c r="H28" s="21">
+        <v>4.3899999999999998E-3</v>
+      </c>
+      <c r="I28" s="2">
+        <v>8.6E-3</v>
+      </c>
+      <c r="J28" s="26">
+        <v>8.9999999999999993E-3</v>
+      </c>
+      <c r="K28" s="28">
+        <v>3.58</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A29">
+        <v>5000</v>
+      </c>
+      <c r="B29" s="9">
+        <v>0.96</v>
+      </c>
+      <c r="C29" s="11">
+        <v>2.76</v>
+      </c>
+      <c r="D29" s="13">
+        <v>0.25600000000000001</v>
+      </c>
+      <c r="E29" s="15">
+        <v>0.121</v>
+      </c>
+      <c r="F29" s="17">
+        <v>0.19600000000000001</v>
+      </c>
+      <c r="G29" s="19">
+        <v>0.159</v>
+      </c>
+      <c r="H29" s="21">
+        <v>6.3899999999999998E-2</v>
+      </c>
+      <c r="I29" s="2">
+        <v>0.17</v>
+      </c>
+      <c r="J29" s="26">
+        <v>0.15</v>
+      </c>
+      <c r="K29" s="28">
+        <v>3.51</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A30">
+        <v>50000</v>
+      </c>
+      <c r="B30" s="9">
+        <v>86.7</v>
+      </c>
+      <c r="C30" s="11">
+        <v>264</v>
+      </c>
+      <c r="D30" s="13">
+        <v>3.7</v>
+      </c>
+      <c r="E30" s="15">
+        <v>1.83</v>
+      </c>
+      <c r="F30" s="17">
+        <v>2.69</v>
+      </c>
+      <c r="G30" s="19">
+        <v>2.0299999999999998</v>
+      </c>
+      <c r="H30" s="21">
+        <v>0.97799999999999998</v>
+      </c>
+      <c r="I30" s="2">
+        <v>1.19</v>
+      </c>
+      <c r="J30" s="26">
+        <v>0.99</v>
+      </c>
+      <c r="K30" s="28">
+        <v>4.3600000000000003</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A31">
+        <v>500000</v>
+      </c>
+      <c r="B31" s="9">
+        <v>10000</v>
+      </c>
+      <c r="C31" s="11">
+        <v>25400</v>
+      </c>
+      <c r="D31" s="13">
+        <v>49.3</v>
+      </c>
+      <c r="E31" s="15">
+        <v>9.84</v>
+      </c>
+      <c r="F31" s="17">
+        <v>33.200000000000003</v>
+      </c>
+      <c r="G31" s="19">
+        <v>26.6</v>
+      </c>
+      <c r="H31" s="21">
+        <v>12.8</v>
+      </c>
+      <c r="I31" s="2">
+        <v>8.4499999999999993</v>
+      </c>
+      <c r="J31" s="26">
+        <v>8.4499999999999993</v>
+      </c>
+      <c r="K31" s="28">
+        <v>5.67</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A32">
+        <v>5000000</v>
+      </c>
+      <c r="B32" s="24">
+        <v>900000</v>
+      </c>
+      <c r="C32" s="24">
+        <v>900000</v>
+      </c>
+      <c r="D32" s="13">
+        <v>626</v>
+      </c>
+      <c r="E32" s="15">
+        <v>604</v>
+      </c>
+      <c r="F32" s="17">
+        <v>384</v>
+      </c>
+      <c r="G32" s="19">
+        <v>320</v>
+      </c>
+      <c r="H32" s="21">
+        <v>138</v>
+      </c>
+      <c r="I32" s="2">
+        <v>79.41</v>
+      </c>
+      <c r="J32" s="26">
+        <v>104</v>
+      </c>
+      <c r="K32" s="28">
+        <v>12.9</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A33">
+        <v>50000000</v>
+      </c>
+      <c r="B33" s="24">
+        <v>900000</v>
+      </c>
+      <c r="C33" s="24">
+        <v>900000</v>
+      </c>
+      <c r="D33" s="13">
+        <v>82800</v>
+      </c>
+      <c r="E33" s="15">
+        <v>30800</v>
+      </c>
+      <c r="F33" s="17">
+        <v>43200</v>
+      </c>
+      <c r="G33" s="19">
+        <v>3400</v>
+      </c>
+      <c r="H33" s="21">
+        <v>1500</v>
+      </c>
+      <c r="I33" s="2">
+        <v>740</v>
+      </c>
+      <c r="J33" s="26">
+        <v>1109</v>
+      </c>
+      <c r="K33" s="28">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A34">
+        <v>500000000</v>
+      </c>
+      <c r="B34" s="24">
+        <v>900000</v>
+      </c>
+      <c r="C34" s="24">
+        <v>900000</v>
+      </c>
+      <c r="D34" s="24">
+        <v>900000</v>
+      </c>
+      <c r="E34" s="24">
+        <v>900000</v>
+      </c>
+      <c r="F34" s="24">
+        <v>900000</v>
+      </c>
+      <c r="G34" s="19">
+        <v>38800</v>
+      </c>
+      <c r="H34" s="21">
+        <v>19400</v>
+      </c>
+      <c r="I34" s="25">
+        <v>8156</v>
+      </c>
+      <c r="J34" s="27">
+        <v>10224</v>
+      </c>
+      <c r="K34" s="29">
+        <v>981</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A35">
+        <v>5000000000</v>
+      </c>
+      <c r="B35" s="24">
+        <v>900000</v>
+      </c>
+      <c r="C35" s="24">
+        <v>900000</v>
+      </c>
+      <c r="D35" s="24">
+        <v>900000</v>
+      </c>
+      <c r="E35" s="24">
+        <v>900000</v>
+      </c>
+      <c r="F35" s="24">
+        <v>900000</v>
+      </c>
+      <c r="G35" s="24">
+        <v>900000</v>
+      </c>
+      <c r="H35" s="24">
+        <v>900000</v>
+      </c>
+      <c r="I35" s="24">
+        <v>900000</v>
+      </c>
+      <c r="J35" s="24">
+        <v>900000</v>
+      </c>
+      <c r="K35" s="29">
+        <v>658669</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>